<commit_message>
Add "Lae12 Hans Win10", strikethrough "Lae12 Hans WinXP"
</commit_message>
<xml_diff>
--- a/docs/disk-usage.xlsx
+++ b/docs/disk-usage.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17030"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Daniela</t>
   </si>
@@ -267,13 +267,19 @@
   </si>
   <si>
     <t>Pra21 Daniela Win10 NTFS 1360GB</t>
+  </si>
+  <si>
+    <t>Lae12 Hans Win10</t>
+  </si>
+  <si>
+    <t>Hans Win10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,6 +314,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -335,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -350,6 +371,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -443,6 +469,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -478,6 +521,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -654,13 +714,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L3" sqref="L3"/>
+      <selection pane="bottomRight" activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,7 +784,7 @@
         <v>1360</v>
       </c>
       <c r="D2" s="5">
-        <f t="shared" ref="D2:D15" si="0">B2/C2</f>
+        <f t="shared" ref="D2:D16" si="0">B2/C2</f>
         <v>0.21102941176470588</v>
       </c>
       <c r="F2">
@@ -953,39 +1013,39 @@
         <v>41483</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="15">
         <v>132</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="15">
         <v>232</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="16">
         <f t="shared" ref="D9" si="1">B9/C9</f>
         <v>0.56896551724137934</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="14">
         <v>140</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J9" t="b">
-        <v>1</v>
-      </c>
-      <c r="K9" t="b">
-        <v>1</v>
-      </c>
-      <c r="L9" s="13">
+      <c r="H9" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="L9" s="18">
         <v>41525</v>
       </c>
     </row>
@@ -1025,165 +1085,193 @@
         <v>41763</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="8">
+        <v>80</v>
+      </c>
+      <c r="C11" s="8">
+        <v>917</v>
+      </c>
+      <c r="D11" s="9">
+        <f t="shared" si="0"/>
+        <v>8.7241003271537623E-2</v>
+      </c>
+      <c r="F11" s="7">
+        <v>140</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11" s="13">
+        <v>42597</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="3">
-        <f>C11-18-2</f>
+      <c r="B12" s="3">
+        <f>C12-18-2</f>
         <v>55</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C12" s="3">
         <f>36+39</f>
         <v>75</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D12" s="9">
         <f t="shared" si="0"/>
         <v>0.73333333333333328</v>
       </c>
-      <c r="F11">
+      <c r="F12">
         <v>30</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G12" t="s">
         <v>23</v>
       </c>
-      <c r="H11" t="b">
-        <v>1</v>
-      </c>
-      <c r="I11" t="b">
-        <v>1</v>
-      </c>
-      <c r="J11" t="b">
-        <v>1</v>
-      </c>
-      <c r="K11" t="b">
-        <v>1</v>
-      </c>
-      <c r="L11" s="12">
+      <c r="H12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" t="b">
+        <v>1</v>
+      </c>
+      <c r="L12" s="12">
         <v>41511</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B13" s="3">
         <v>55</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C13" s="3">
         <v>500</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D13" s="9">
         <f t="shared" si="0"/>
         <v>0.11</v>
       </c>
-      <c r="F12">
+      <c r="F13">
         <v>100</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G13" t="s">
         <v>35</v>
       </c>
-      <c r="H12" t="b">
-        <v>1</v>
-      </c>
-      <c r="I12" t="b">
-        <v>1</v>
-      </c>
-      <c r="J12" t="b">
-        <v>1</v>
-      </c>
-      <c r="K12" t="b">
-        <v>1</v>
-      </c>
-      <c r="L12" s="12">
+      <c r="H13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13" t="b">
+        <v>1</v>
+      </c>
+      <c r="L13" s="12">
         <v>41780</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C14" s="3">
         <v>500</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D14" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F13">
+      <c r="F14">
         <v>100</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G14" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="H13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K13" t="b">
-        <v>1</v>
-      </c>
-      <c r="L13" s="12">
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" t="b">
+        <v>1</v>
+      </c>
+      <c r="L14" s="12">
         <v>41290</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="3">
-        <f>C14-356</f>
+      <c r="B15" s="3">
+        <f>C15-356</f>
         <v>91</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C15" s="3">
         <v>447</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D15" s="5">
         <f t="shared" si="0"/>
         <v>0.20357941834451901</v>
       </c>
-      <c r="F14">
+      <c r="F15">
         <v>150</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G15" t="s">
         <v>30</v>
       </c>
-      <c r="L14" s="12">
+      <c r="L15" s="12">
         <v>41300</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B16" s="3">
         <v>50</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C16" s="3">
         <v>915</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D16" s="5">
         <f t="shared" si="0"/>
         <v>5.4644808743169397E-2</v>
       </c>
-      <c r="F15">
+      <c r="F16">
         <v>100</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G16" t="s">
         <v>37</v>
       </c>
-      <c r="J15" t="b">
-        <v>1</v>
-      </c>
-      <c r="K15" t="b">
-        <v>1</v>
-      </c>
-      <c r="L15" s="12">
+      <c r="J16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K16" t="b">
+        <v>1</v>
+      </c>
+      <c r="L16" s="12">
         <v>42128</v>
       </c>
     </row>

</xml_diff>